<commit_message>
Final Version of Code before Submission
</commit_message>
<xml_diff>
--- a/Final Project/Case Study Data/case1.xlsx
+++ b/Final Project/Case Study Data/case1.xlsx
@@ -42,7 +42,7 @@
     <t>eps0xy</t>
   </si>
   <si>
-    <t>Local Stress</t>
+    <t>Global Stress</t>
   </si>
   <si>
     <t>sigma1</t>
@@ -54,7 +54,7 @@
     <t>sigma12</t>
   </si>
   <si>
-    <t>Local Strain</t>
+    <t>Global Strain</t>
   </si>
   <si>
     <t>epsilon1</t>
@@ -134,15 +134,15 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.28515625" customWidth="true"/>
-    <col min="2" max="2" width="16.42578125" customWidth="true"/>
-    <col min="3" max="3" width="13.42578125" customWidth="true"/>
-    <col min="4" max="4" width="12.7109375" customWidth="true"/>
-    <col min="5" max="5" width="13.42578125" customWidth="true"/>
-    <col min="6" max="6" width="16.42578125" customWidth="true"/>
-    <col min="7" max="7" width="13.42578125" customWidth="true"/>
-    <col min="8" max="8" width="12.42578125" customWidth="true"/>
-    <col min="9" max="9" width="12.7109375" customWidth="true"/>
-    <col min="10" max="10" width="12.7109375" customWidth="true"/>
+    <col min="2" max="2" width="16.28515625" customWidth="true"/>
+    <col min="3" max="3" width="15.42578125" customWidth="true"/>
+    <col min="4" max="4" width="15.7109375" customWidth="true"/>
+    <col min="5" max="5" width="15.42578125" customWidth="true"/>
+    <col min="6" max="6" width="14.7109375" customWidth="true"/>
+    <col min="7" max="7" width="15.7109375" customWidth="true"/>
+    <col min="8" max="8" width="15.42578125" customWidth="true"/>
+    <col min="9" max="9" width="15.5703125" customWidth="true"/>
+    <col min="10" max="10" width="16.42578125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -150,7 +150,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0">
-        <v>-4.023827331946249</v>
+        <v>-102.20515904064884</v>
       </c>
       <c r="C1" s="0"/>
       <c r="D1" s="0" t="s">
@@ -174,7 +174,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0">
-        <v>5.976172668053751</v>
+        <v>-92.205159040648851</v>
       </c>
       <c r="C2" s="0"/>
       <c r="D2" s="0" t="s">
@@ -194,7 +194,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0">
-        <v>0</v>
+        <v>1.4988010832439613e-14</v>
       </c>
       <c r="C3" s="0"/>
       <c r="D3" s="0" t="s">
@@ -258,31 +258,31 @@
         <v>4</v>
       </c>
       <c r="B6" s="0">
-        <v>-0.00078740199999999998</v>
+        <v>-0.02</v>
       </c>
       <c r="C6" s="0">
-        <v>-0.00059055149999999999</v>
+        <v>-0.014999999999999999</v>
       </c>
       <c r="D6" s="0">
-        <v>-0.00039370099999999999</v>
+        <v>-0.01</v>
       </c>
       <c r="E6" s="0">
-        <v>-0.0001968505</v>
+        <v>-0.0050000000000000001</v>
       </c>
       <c r="F6" s="0">
         <v>0</v>
       </c>
       <c r="G6" s="0">
-        <v>0.0001968505</v>
+        <v>0.0050000000000000001</v>
       </c>
       <c r="H6" s="0">
-        <v>0.00039370099999999999</v>
+        <v>0.01</v>
       </c>
       <c r="I6" s="0">
-        <v>0.00059055149999999999</v>
+        <v>0.014999999999999999</v>
       </c>
       <c r="J6" s="0">
-        <v>0.00078740199999999998</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="7">
@@ -316,14 +316,14 @@
         <v>6</v>
       </c>
       <c r="B9" s="0">
-        <v>-0.00023083241951707544</v>
+        <v>-9.087895439630704e-06</v>
       </c>
       <c r="C9" s="0"/>
       <c r="D9" s="0" t="s">
         <v>20</v>
       </c>
       <c r="E9" s="0">
-        <v>3757.9564816486577</v>
+        <v>0.2293249461612798</v>
       </c>
       <c r="F9" s="0"/>
       <c r="G9" s="0"/>
@@ -336,14 +336,14 @@
         <v>7</v>
       </c>
       <c r="B10" s="0">
-        <v>0.00079497582297084312</v>
+        <v>3.129827764794541e-05</v>
       </c>
       <c r="C10" s="0"/>
       <c r="D10" s="0" t="s">
         <v>21</v>
       </c>
       <c r="E10" s="0">
-        <v>-1834.0126929041348</v>
+        <v>-0.11191850254605111</v>
       </c>
       <c r="F10" s="0"/>
       <c r="G10" s="0"/>
@@ -356,14 +356,14 @@
         <v>8</v>
       </c>
       <c r="B11" s="0">
-        <v>-1.2293164912577145e-17</v>
+        <v>-1.7732260743946512e-20</v>
       </c>
       <c r="C11" s="0"/>
       <c r="D11" s="0" t="s">
         <v>22</v>
       </c>
       <c r="E11" s="0">
-        <v>-539.70606421731031</v>
+        <v>-0.032934938103714423</v>
       </c>
       <c r="F11" s="0"/>
       <c r="G11" s="0"/>
@@ -402,31 +402,31 @@
         <v>10</v>
       </c>
       <c r="B14" s="0">
-        <v>-11393115.006010905</v>
+        <v>-16889.701725295057</v>
       </c>
       <c r="C14" s="0">
-        <v>-14820210.880334646</v>
+        <v>-17244.851983221826</v>
       </c>
       <c r="D14" s="0">
-        <v>13895332.126171283</v>
+        <v>2640.636991605913</v>
       </c>
       <c r="E14" s="0">
-        <v>-14740891.836667251</v>
+        <v>-28614.729409363455</v>
       </c>
       <c r="F14" s="0">
-        <v>-9910.3705420509996</v>
+        <v>-5781.6378110165651</v>
       </c>
       <c r="G14" s="0">
-        <v>14721071.095583148</v>
+        <v>17051.453787330327</v>
       </c>
       <c r="H14" s="0">
-        <v>-13874758.20137177</v>
+        <v>8584.1833227775278</v>
       </c>
       <c r="I14" s="0">
-        <v>14820587.472192351</v>
+        <v>17414.079637046674</v>
       </c>
       <c r="J14" s="0">
-        <v>11393491.59786861</v>
+        <v>17058.929379119905</v>
       </c>
     </row>
     <row r="15">
@@ -434,31 +434,31 @@
         <v>11</v>
       </c>
       <c r="B15" s="0">
-        <v>-1696554.7623164279</v>
+        <v>-3159.1914308266714</v>
       </c>
       <c r="C15" s="0">
-        <v>-929279.7298736783</v>
+        <v>-6926.7761758267479</v>
       </c>
       <c r="D15" s="0">
-        <v>-1911655.1144042811</v>
+        <v>16535.419497826042</v>
       </c>
       <c r="E15" s="0">
-        <v>227852.03734683868</v>
+        <v>5998.4634740204856</v>
       </c>
       <c r="F15" s="0">
-        <v>6711.4108282734951</v>
+        <v>5655.6944471891475</v>
       </c>
       <c r="G15" s="0">
-        <v>-214429.21569029166</v>
+        <v>5312.9254203578093</v>
       </c>
       <c r="H15" s="0">
-        <v>1922879.0953163328</v>
+        <v>-26508.353084554634</v>
       </c>
       <c r="I15" s="0">
-        <v>941603.13115797879</v>
+        <v>7257.5485220019</v>
       </c>
       <c r="J15" s="0">
-        <v>1708878.1636007281</v>
+        <v>3489.9637770018235</v>
       </c>
     </row>
     <row r="16">
@@ -466,31 +466,31 @@
         <v>12</v>
       </c>
       <c r="B16" s="0">
-        <v>4404153.520223707</v>
+        <v>-13019.280233880081</v>
       </c>
       <c r="C16" s="0">
-        <v>-3303371.5922284019</v>
+        <v>16269.927698608441</v>
       </c>
       <c r="D16" s="0">
-        <v>-212482.81718841926</v>
+        <v>329.34938103714438</v>
       </c>
       <c r="E16" s="0">
-        <v>106241.40859420961</v>
+        <v>164.67469051857225</v>
       </c>
       <c r="F16" s="0">
-        <v>-1.2293164912577146e-11</v>
+        <v>1.5669259898113025e-13</v>
       </c>
       <c r="G16" s="0">
-        <v>-106241.40859420964</v>
+        <v>-164.67469051857196</v>
       </c>
       <c r="H16" s="0">
-        <v>212482.81718841926</v>
+        <v>-329.34938103714404</v>
       </c>
       <c r="I16" s="0">
-        <v>3301319.9757434265</v>
+        <v>-5251.8230942275768</v>
       </c>
       <c r="J16" s="0">
-        <v>-4402101.9037387315</v>
+        <v>2001.1756294992174</v>
       </c>
     </row>
     <row r="17">
@@ -524,31 +524,31 @@
         <v>14</v>
       </c>
       <c r="B19" s="0">
-        <v>-0.54505570624695687</v>
+        <v>-0.0028650883832606671</v>
       </c>
       <c r="C19" s="0">
-        <v>-0.72753598793356378</v>
+        <v>-0.0017184636524542691</v>
       </c>
       <c r="D19" s="0">
-        <v>0.72248560546742613</v>
+        <v>0.0015206610783521312</v>
       </c>
       <c r="E19" s="0">
-        <v>-0.74034844637489161</v>
+        <v>-0.0015177141908414697</v>
       </c>
       <c r="F19" s="0">
-        <v>-0.00059283398411251562</v>
+        <v>-0.00037108946003507087</v>
       </c>
       <c r="G19" s="0">
-        <v>0.73916277840666655</v>
+        <v>0.00077553527077132804</v>
       </c>
       <c r="H19" s="0">
-        <v>-0.72161965695067531</v>
+        <v>0.006107160001577727</v>
       </c>
       <c r="I19" s="0">
-        <v>0.72737612820782749</v>
+        <v>0.0051612847323841268</v>
       </c>
       <c r="J19" s="0">
-        <v>0.54489584652121981</v>
+        <v>0.0063079094631905246</v>
       </c>
     </row>
     <row r="20">
@@ -556,31 +556,31 @@
         <v>15</v>
       </c>
       <c r="B20" s="0">
-        <v>-0.96583634062379464</v>
+        <v>0.004000166763973528</v>
       </c>
       <c r="C20" s="0">
-        <v>-0.40462676215093429</v>
+        <v>0.0034405742512432719</v>
       </c>
       <c r="D20" s="0">
-        <v>-1.475919058765671</v>
+        <v>0.0007884817385130162</v>
       </c>
       <c r="E20" s="0">
-        <v>0.36564428986290093</v>
+        <v>0.0044138892257827604</v>
       </c>
       <c r="F20" s="0">
-        <v>0.0046179742583754031</v>
+        <v>0.0038542967130525047</v>
       </c>
       <c r="G20" s="0">
-        <v>-0.35640834134615007</v>
+        <v>0.0032947042003222491</v>
       </c>
       <c r="H20" s="0">
-        <v>1.483103390797446</v>
+        <v>-0.001449888312408006</v>
       </c>
       <c r="I20" s="0">
-        <v>0.41283690242519799</v>
+        <v>8.3019174861737651e-05</v>
       </c>
       <c r="J20" s="0">
-        <v>0.97404648089805801</v>
+        <v>-0.00047657333786851907</v>
       </c>
     </row>
     <row r="21">
@@ -588,31 +588,31 @@
         <v>16</v>
       </c>
       <c r="B21" s="0">
-        <v>4.4041535202237085</v>
+        <v>-0.0035263012379257129</v>
       </c>
       <c r="C21" s="0">
-        <v>-3.3033715922284035</v>
+        <v>0.0046790240715557166</v>
       </c>
       <c r="D21" s="0">
-        <v>-0.21248281718841924</v>
+        <v>0.00032934938103714438</v>
       </c>
       <c r="E21" s="0">
-        <v>0.10624140859420961</v>
+        <v>0.00016467469051857224</v>
       </c>
       <c r="F21" s="0">
-        <v>-1.2293164912577145e-17</v>
+        <v>1.5669259898113025e-19</v>
       </c>
       <c r="G21" s="0">
-        <v>-0.10624140859420964</v>
+        <v>-0.00016467469051857197</v>
       </c>
       <c r="H21" s="0">
-        <v>0.21248281718841924</v>
+        <v>-0.00032934938103714405</v>
       </c>
       <c r="I21" s="0">
-        <v>3.3013199757434286</v>
+        <v>0.0036909759284442824</v>
       </c>
       <c r="J21" s="0">
-        <v>-4.4021019037387328</v>
+        <v>-0.0048436987620742843</v>
       </c>
     </row>
   </sheetData>

</xml_diff>